<commit_message>
Made it a bit more accurate when it comes to total spendings of any category
</commit_message>
<xml_diff>
--- a/data/1/samplepnl.xlsx
+++ b/data/1/samplepnl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28rac\Desktop\hybrid_chatbot\data\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C65033-620D-4FB0-A720-8C286414628A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E0B26A-AF27-4D2C-B3CD-74C57B991B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="3810" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="2850" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <r>
       <rPr>
@@ -770,6 +770,9 @@
   </si>
   <si>
     <t>Advertising &amp; marketing</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -1301,7 +1304,7 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1348,7 +1351,9 @@
       <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:7" ht="12.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>